<commit_message>
changed database tables and .sql file per discussion
</commit_message>
<xml_diff>
--- a/db/upkeep.xlsx
+++ b/db/upkeep.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="27960" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="27960" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>Dishwasher</t>
   </si>
@@ -130,15 +130,6 @@
     <t>SERIAL123456</t>
   </si>
   <si>
-    <t>estimated_life</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>remaining_life</t>
-  </si>
-  <si>
     <t>tasks</t>
   </si>
   <si>
@@ -157,9 +148,6 @@
     <t>task_frequency</t>
   </si>
   <si>
-    <t>time_remaining</t>
-  </si>
-  <si>
     <t>users</t>
   </si>
   <si>
@@ -185,6 +173,15 @@
   </si>
   <si>
     <t>jkl@aol.com</t>
+  </si>
+  <si>
+    <t>items_note</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Integer nec odio. Praesent libero. Sed cursus ante dapibus diam. Sed nisi. Nulla quis sem at nibh elementum imperdiet. Duis sagittis ipsum. Praesent mauris. Fusce nec tellus sed augue semper porta.</t>
+  </si>
+  <si>
+    <t>task_note</t>
   </si>
 </sst>
 </file>
@@ -331,7 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -397,9 +394,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -747,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K10"/>
+  <dimension ref="B1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -762,30 +756,26 @@
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="216" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B2" s="24" t="s">
+    <row r="1" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B2" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
       <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="26"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>25</v>
@@ -803,19 +793,13 @@
         <v>29</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="5">
         <v>1</v>
       </c>
@@ -835,21 +819,13 @@
         <v>30</v>
       </c>
       <c r="H4" s="6">
-        <v>8</v>
-      </c>
-      <c r="I4" s="6">
-        <f t="shared" ref="I4:I10" ca="1" si="0">DATEDIF(F4,NOW(),"y")</f>
-        <v>5</v>
-      </c>
-      <c r="J4" s="6">
-        <f ca="1">H4-I4</f>
-        <v>3</v>
-      </c>
-      <c r="K4" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I4" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="5">
         <v>2</v>
       </c>
@@ -869,21 +845,13 @@
         <v>12153232523</v>
       </c>
       <c r="H5" s="6">
-        <v>7</v>
-      </c>
-      <c r="I5" s="6">
-        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
-      <c r="J5" s="6">
-        <f t="shared" ref="J5:J10" ca="1" si="1">H5-I5</f>
-        <v>6</v>
-      </c>
-      <c r="K5" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I5" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="5">
         <v>3</v>
       </c>
@@ -903,21 +871,13 @@
         <v>31</v>
       </c>
       <c r="H6" s="6">
-        <v>7</v>
-      </c>
-      <c r="I6" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="J6" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="K6" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I6" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="5">
         <v>4</v>
       </c>
@@ -937,21 +897,13 @@
         <v>998182951</v>
       </c>
       <c r="H7" s="6">
-        <v>14</v>
-      </c>
-      <c r="I7" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="J7" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="K7" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I7" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
         <v>5</v>
       </c>
@@ -971,21 +923,13 @@
         <v>32</v>
       </c>
       <c r="H8" s="6">
-        <v>12</v>
-      </c>
-      <c r="I8" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="J8" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="K8" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I8" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
         <v>6</v>
       </c>
@@ -1005,21 +949,13 @@
         <v>77261747716282</v>
       </c>
       <c r="H9" s="6">
-        <v>9</v>
-      </c>
-      <c r="I9" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J9" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="K9" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9">
         <v>7</v>
       </c>
@@ -1039,23 +975,15 @@
         <v>33</v>
       </c>
       <c r="H10" s="10">
-        <v>11</v>
-      </c>
-      <c r="I10" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J10" s="10">
-        <f t="shared" ca="1" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="K10" s="12">
         <v>2</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1066,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6FC2EAF-C471-864D-9379-FF13F550B3B1}">
   <dimension ref="B1:K8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1078,7 +1006,8 @@
     <col min="4" max="4" width="18.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="19" style="1" customWidth="1"/>
     <col min="6" max="6" width="24" style="1" customWidth="1"/>
-    <col min="7" max="8" width="23.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="213.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="16.83203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="16.5" style="1" customWidth="1"/>
@@ -1086,38 +1015,38 @@
   <sheetData>
     <row r="1" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
+      <c r="B2" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
       <c r="I2" s="13"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="H3" s="4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
@@ -1136,12 +1065,11 @@
       <c r="F4" s="6">
         <v>182</v>
       </c>
-      <c r="G4" s="16">
-        <f ca="1">(F4)-DATEDIF(E4,NOW(),"d")</f>
-        <v>112</v>
-      </c>
-      <c r="H4" s="8">
+      <c r="G4" s="6">
         <v>1</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1160,12 +1088,11 @@
       <c r="F5" s="14">
         <v>1825</v>
       </c>
-      <c r="G5" s="16">
-        <f ca="1">(F5)-DATEDIF(E5,NOW(),"d")</f>
-        <v>755</v>
-      </c>
-      <c r="H5" s="8">
+      <c r="G5" s="6">
         <v>1</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1184,12 +1111,11 @@
       <c r="F6" s="6">
         <v>365</v>
       </c>
-      <c r="G6" s="16">
-        <f t="shared" ref="G6:G8" ca="1" si="0">(F6)-DATEDIF(E6,NOW(),"d")</f>
-        <v>351</v>
-      </c>
-      <c r="H6" s="8">
+      <c r="G6" s="6">
         <v>1</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1208,12 +1134,11 @@
       <c r="F7" s="6">
         <v>730</v>
       </c>
-      <c r="G7" s="16">
-        <f t="shared" ca="1" si="0"/>
-        <v>-417</v>
-      </c>
-      <c r="H7" s="8">
+      <c r="G7" s="6">
         <v>1</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:9" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1232,12 +1157,11 @@
       <c r="F8" s="15">
         <v>1825</v>
       </c>
-      <c r="G8" s="23">
-        <f t="shared" ca="1" si="0"/>
-        <v>878</v>
-      </c>
-      <c r="H8" s="12">
+      <c r="G8" s="10">
         <v>2</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1278,24 +1202,24 @@
   <sheetData>
     <row r="1" spans="2:7" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26"/>
+      <c r="B2" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
     </row>
     <row r="3" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="3"/>
@@ -1306,7 +1230,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D4" s="18">
         <v>43101</v>
@@ -1320,7 +1244,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D5" s="18">
         <v>43103</v>
@@ -1334,7 +1258,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D6" s="18">
         <v>43106</v>
@@ -1348,7 +1272,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D7" s="18">
         <v>43112</v>
@@ -1362,7 +1286,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D8" s="19">
         <v>43120</v>

</xml_diff>